<commit_message>
Check file fully working
Could still do with a bit of tidying - better to be consistent and convert all H5 refs to paths in code. Only bit to keep as refs is bit to find unique ones as this should be possible without dereferencing, although at present that is exactly how it is done, followed by identifying unique paths and converting back to refs!
</commit_message>
<xml_diff>
--- a/MFMC Specification 2.0.0.xlsx
+++ b/MFMC Specification 2.0.0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mepdw\Git\MFMCPy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA3C3B1D-4FE1-4126-B182-D69983EB5D07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA11BBE1-4B97-460A-BAC0-F2CF3DC35752}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{4EB7791A-BAE0-498A-A1B8-D04CCDD529C8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4EB7791A-BAE0-498A-A1B8-D04CCDD529C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="87">
   <si>
     <t>Name</t>
   </si>
@@ -74,15 +74,9 @@
     <t>“2.0.0”</t>
   </si>
   <si>
-    <t>/{probe}/TYPE</t>
-  </si>
-  <si>
     <t>“PROBE”</t>
   </si>
   <si>
-    <t>/{probe}/ELEMENT_POSITION</t>
-  </si>
-  <si>
     <t>D</t>
   </si>
   <si>
@@ -92,192 +86,60 @@
     <t>[3,N_E&lt;p&gt;]</t>
   </si>
   <si>
-    <t>/{probe}/ELEMENT_MINOR</t>
-  </si>
-  <si>
-    <t>/{probe}/ELEMENT_MAJOR</t>
-  </si>
-  <si>
-    <t>/{probe}/ELEMENT_SHAPE</t>
-  </si>
-  <si>
     <t>H5T_INTEGER</t>
   </si>
   <si>
     <t>[N_E&lt;p&gt;]</t>
   </si>
   <si>
-    <t>/{probe}/ELEMENT_RADIUS_OF_CURVATURE</t>
-  </si>
-  <si>
     <t>O</t>
   </si>
   <si>
-    <t>/{probe}/ELEMENT_AXIS_OF_CURVATURE</t>
-  </si>
-  <si>
-    <t>/{probe}/WEDGE_SURFACE_POINT</t>
-  </si>
-  <si>
     <t>[3]</t>
   </si>
   <si>
-    <t>/{probe}/WEDGE_SURFACE_NORMAL</t>
-  </si>
-  <si>
-    <t>/{probe}/DEAD_ELEMENT</t>
-  </si>
-  <si>
-    <t>/{probe}/CENTRE_FREQUENCY</t>
-  </si>
-  <si>
     <t>[1]</t>
   </si>
   <si>
-    <t>/{probe}/BANDWIDTH</t>
-  </si>
-  <si>
     <t>/TYPE</t>
   </si>
   <si>
-    <t>/{probe}/PROBE_MANUFACTURER</t>
-  </si>
-  <si>
-    <t>/{probe}/PROBE_SERIAL_NUMBER</t>
-  </si>
-  <si>
-    <t>/{probe}/PROBE_TAG</t>
-  </si>
-  <si>
-    <t>/{probe}/WEDGE_MANUFACTURER</t>
-  </si>
-  <si>
-    <t>/{probe}/WEDGE_SERIAL_NUMBER</t>
-  </si>
-  <si>
-    <t>/{probe}/WEDGE_TAG</t>
-  </si>
-  <si>
-    <t>/{sequence}/TYPE</t>
-  </si>
-  <si>
     <t>“SEQUENCE”</t>
   </si>
   <si>
-    <t>/{sequence}/MFMC_DATA</t>
-  </si>
-  <si>
     <t>H5T_FLOAT / H5T_INTEGER</t>
   </si>
   <si>
     <t>[N_T&lt;m&gt;,N_A&lt;m&gt;,N_F&lt;m&gt;]</t>
   </si>
   <si>
-    <t>/{sequence}/MFMC_DATA_IM</t>
-  </si>
-  <si>
-    <t>/{sequence}/PROBE_PLACEMENT_INDEX</t>
-  </si>
-  <si>
     <t>[N_A&lt;m&gt;,N_F&lt;m&gt;]</t>
   </si>
   <si>
-    <t>/{sequence}/PROBE_POSITION</t>
-  </si>
-  <si>
     <t>[3,N_Q&lt;m&gt;,N_B&lt;m&gt;]</t>
   </si>
   <si>
-    <t>/{sequence}/PROBE_X_DIRECTION</t>
-  </si>
-  <si>
-    <t>/{sequence}/PROBE_Y_DIRECTION</t>
-  </si>
-  <si>
-    <t>/{sequence}/TRANSMIT_LAW</t>
-  </si>
-  <si>
     <t>H5T_STD_REF_OBJ</t>
   </si>
   <si>
     <t>[N_A&lt;m&gt;]</t>
   </si>
   <si>
-    <t>/{sequence}/RECEIVE_LAW</t>
-  </si>
-  <si>
-    <t>/{sequence}/PROBE_LIST</t>
-  </si>
-  <si>
     <t>[N_Q&lt;m&gt;]</t>
   </si>
   <si>
-    <t>/{sequence}/TIME_STEP</t>
-  </si>
-  <si>
-    <t>/{sequence}/START_TIME</t>
-  </si>
-  <si>
-    <t>/{sequence}/SPECIMEN_VELOCITY</t>
-  </si>
-  <si>
     <t>[2]</t>
   </si>
   <si>
-    <t>/{sequence}/WEDGE_VELOCITY</t>
-  </si>
-  <si>
-    <t>/{sequence}/TAG</t>
-  </si>
-  <si>
-    <t>/{sequence}/DAC_CURVE</t>
-  </si>
-  <si>
     <t>[N_T&lt;m&gt;]</t>
   </si>
   <si>
-    <t>/{sequence}/RECEIVER_AMPLIFIER_GAIN</t>
-  </si>
-  <si>
-    <t>/{sequence}/FILTER_TYPE</t>
-  </si>
-  <si>
-    <t>/{sequence}/FILTER_PARAMETERS</t>
-  </si>
-  <si>
     <t>[3,N_F&lt;m&gt;]</t>
   </si>
   <si>
-    <t>/{sequence}/FILTER_DESCRIPTION</t>
-  </si>
-  <si>
-    <t>/{sequence}/OPERATOR</t>
-  </si>
-  <si>
-    <t>/{sequence}/DATE_AND_TIME</t>
-  </si>
-  <si>
     <t>“LAW”</t>
   </si>
   <si>
-    <t>[N_C&lt;m&gt;&lt;k&gt;]</t>
-  </si>
-  <si>
-    <t>/{law}/TYPE</t>
-  </si>
-  <si>
-    <t>/{law}/PROBE</t>
-  </si>
-  <si>
-    <t>/{law}/ELEMENT</t>
-  </si>
-  <si>
-    <t>/{law}/DELAY</t>
-  </si>
-  <si>
-    <t>/{law}/WEIGHTING</t>
-  </si>
-  <si>
     <t>Reference to</t>
   </si>
   <si>
@@ -285,6 +147,156 @@
   </si>
   <si>
     <t>PROBE</t>
+  </si>
+  <si>
+    <t>[N_C&lt;k&gt;]</t>
+  </si>
+  <si>
+    <t>{law}/PROBE</t>
+  </si>
+  <si>
+    <t>{law}/ELEMENT</t>
+  </si>
+  <si>
+    <t>{law}/DELAY</t>
+  </si>
+  <si>
+    <t>{law}/WEIGHTING</t>
+  </si>
+  <si>
+    <t>{probe}/TYPE</t>
+  </si>
+  <si>
+    <t>{probe}/ELEMENT_POSITION</t>
+  </si>
+  <si>
+    <t>{probe}/ELEMENT_MINOR</t>
+  </si>
+  <si>
+    <t>{probe}/ELEMENT_MAJOR</t>
+  </si>
+  <si>
+    <t>{probe}/ELEMENT_SHAPE</t>
+  </si>
+  <si>
+    <t>{probe}/ELEMENT_RADIUS_OF_CURVATURE</t>
+  </si>
+  <si>
+    <t>{probe}/ELEMENT_AXIS_OF_CURVATURE</t>
+  </si>
+  <si>
+    <t>{probe}/WEDGE_SURFACE_POINT</t>
+  </si>
+  <si>
+    <t>{probe}/WEDGE_SURFACE_NORMAL</t>
+  </si>
+  <si>
+    <t>{probe}/DEAD_ELEMENT</t>
+  </si>
+  <si>
+    <t>{probe}/CENTRE_FREQUENCY</t>
+  </si>
+  <si>
+    <t>{probe}/BANDWIDTH</t>
+  </si>
+  <si>
+    <t>{probe}/PROBE_MANUFACTURER</t>
+  </si>
+  <si>
+    <t>{probe}/PROBE_SERIAL_NUMBER</t>
+  </si>
+  <si>
+    <t>{probe}/PROBE_TAG</t>
+  </si>
+  <si>
+    <t>{probe}/WEDGE_MANUFACTURER</t>
+  </si>
+  <si>
+    <t>{probe}/WEDGE_SERIAL_NUMBER</t>
+  </si>
+  <si>
+    <t>{probe}/WEDGE_TAG</t>
+  </si>
+  <si>
+    <t>{sequence}/TYPE</t>
+  </si>
+  <si>
+    <t>{sequence}/MFMC_DATA</t>
+  </si>
+  <si>
+    <t>{sequence}/MFMC_DATA_IM</t>
+  </si>
+  <si>
+    <t>{sequence}/PROBE_PLACEMENT_INDEX</t>
+  </si>
+  <si>
+    <t>{sequence}/PROBE_POSITION</t>
+  </si>
+  <si>
+    <t>{sequence}/PROBE_X_DIRECTION</t>
+  </si>
+  <si>
+    <t>{sequence}/PROBE_Y_DIRECTION</t>
+  </si>
+  <si>
+    <t>{sequence}/TRANSMIT_LAW</t>
+  </si>
+  <si>
+    <t>{sequence}/RECEIVE_LAW</t>
+  </si>
+  <si>
+    <t>{sequence}/PROBE_LIST</t>
+  </si>
+  <si>
+    <t>{sequence}/TIME_STEP</t>
+  </si>
+  <si>
+    <t>{sequence}/START_TIME</t>
+  </si>
+  <si>
+    <t>{sequence}/SPECIMEN_VELOCITY</t>
+  </si>
+  <si>
+    <t>{sequence}/WEDGE_VELOCITY</t>
+  </si>
+  <si>
+    <t>{sequence}/TAG</t>
+  </si>
+  <si>
+    <t>{sequence}/DAC_CURVE</t>
+  </si>
+  <si>
+    <t>{sequence}/RECEIVER_AMPLIFIER_GAIN</t>
+  </si>
+  <si>
+    <t>{sequence}/FILTER_TYPE</t>
+  </si>
+  <si>
+    <t>{sequence}/FILTER_PARAMETERS</t>
+  </si>
+  <si>
+    <t>{sequence}/FILTER_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>{sequence}/OPERATOR</t>
+  </si>
+  <si>
+    <t>{sequence}/DATE_AND_TIME</t>
+  </si>
+  <si>
+    <t>{law}/TYPE</t>
+  </si>
+  <si>
+    <t>{sequence}/VERSION</t>
+  </si>
+  <si>
+    <t>Maximum</t>
+  </si>
+  <si>
+    <t>N_B&lt;m&gt;</t>
+  </si>
+  <si>
+    <t>N_E&lt;{law}/PROBE&gt;</t>
   </si>
 </sst>
 </file>
@@ -636,23 +648,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6FFC392-8FA7-48F3-8553-CFA6D470B666}">
-  <dimension ref="A1:G48"/>
+  <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -672,15 +685,18 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+        <v>34</v>
+      </c>
+      <c r="H1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
@@ -695,12 +711,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
@@ -715,9 +731,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -732,192 +748,192 @@
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E5">
         <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E6">
         <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E7">
         <v>2</v>
       </c>
       <c r="F7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E9">
         <v>1</v>
       </c>
       <c r="F9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E10">
         <v>2</v>
       </c>
       <c r="F10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-      <c r="F11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="F12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="F13" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="B14" t="s">
         <v>6</v>
@@ -926,41 +942,41 @@
         <v>7</v>
       </c>
       <c r="D14" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E14">
         <v>1</v>
       </c>
       <c r="F14" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C15" t="s">
         <v>7</v>
       </c>
       <c r="D15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E15">
         <v>1</v>
       </c>
       <c r="F15" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="B16" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C16" t="s">
         <v>7</v>
@@ -972,15 +988,15 @@
         <v>1</v>
       </c>
       <c r="F16" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="B17" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C17" t="s">
         <v>7</v>
@@ -992,15 +1008,15 @@
         <v>1</v>
       </c>
       <c r="F17" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="B18" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C18" t="s">
         <v>7</v>
@@ -1012,15 +1028,15 @@
         <v>1</v>
       </c>
       <c r="F18" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="B19" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C19" t="s">
         <v>7</v>
@@ -1032,15 +1048,15 @@
         <v>1</v>
       </c>
       <c r="F19" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="B20" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C20" t="s">
         <v>7</v>
@@ -1052,15 +1068,15 @@
         <v>1</v>
       </c>
       <c r="F20" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="B21" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C21" t="s">
         <v>7</v>
@@ -1072,12 +1088,12 @@
         <v>1</v>
       </c>
       <c r="F21" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="B22" t="s">
         <v>6</v>
@@ -1092,221 +1108,224 @@
         <v>1</v>
       </c>
       <c r="F22" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>42</v>
+        <v>83</v>
       </c>
       <c r="B23" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C23" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="D23" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="E23">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F23" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="B24" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="C24" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D24" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="E24">
         <v>3</v>
       </c>
       <c r="F24" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="B25" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C25" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D25" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E25">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F25" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="B26" t="s">
         <v>6</v>
       </c>
       <c r="C26" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D26" t="s">
         <v>16</v>
       </c>
       <c r="E26">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F26" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+      <c r="H26" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="B27" t="s">
         <v>6</v>
       </c>
       <c r="C27" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D27" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E27">
         <v>3</v>
       </c>
       <c r="F27" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="B28" t="s">
         <v>6</v>
       </c>
       <c r="C28" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D28" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E28">
         <v>3</v>
       </c>
       <c r="F28" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="B29" t="s">
         <v>6</v>
       </c>
       <c r="C29" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D29" t="s">
-        <v>53</v>
+        <v>14</v>
       </c>
       <c r="E29">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F29" t="s">
-        <v>54</v>
-      </c>
-      <c r="G29" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="B30" t="s">
         <v>6</v>
       </c>
       <c r="C30" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D30" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
       <c r="E30">
         <v>1</v>
       </c>
       <c r="F30" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
       <c r="G30" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="B31" t="s">
         <v>6</v>
       </c>
       <c r="C31" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D31" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
       <c r="E31">
         <v>1</v>
       </c>
       <c r="F31" t="s">
-        <v>57</v>
+        <v>28</v>
       </c>
       <c r="G31" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="B32" t="s">
         <v>6</v>
       </c>
       <c r="C32" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D32" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="E32">
         <v>1</v>
       </c>
       <c r="F32" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+        <v>29</v>
+      </c>
+      <c r="G32" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="B33" t="s">
         <v>6</v>
@@ -1315,18 +1334,18 @@
         <v>7</v>
       </c>
       <c r="D33" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E33">
         <v>1</v>
       </c>
       <c r="F33" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="B34" t="s">
         <v>6</v>
@@ -1335,87 +1354,87 @@
         <v>7</v>
       </c>
       <c r="D34" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E34">
         <v>1</v>
       </c>
       <c r="F34" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="B35" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="C35" t="s">
         <v>7</v>
       </c>
       <c r="D35" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E35">
         <v>1</v>
       </c>
       <c r="F35" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="B36" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C36" t="s">
         <v>7</v>
       </c>
       <c r="D36" t="s">
+        <v>14</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="F36" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>74</v>
+      </c>
+      <c r="B37" t="s">
+        <v>18</v>
+      </c>
+      <c r="C37" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" t="s">
         <v>8</v>
       </c>
-      <c r="E36">
-        <v>1</v>
-      </c>
-      <c r="F36" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>64</v>
-      </c>
-      <c r="B37" t="s">
-        <v>24</v>
-      </c>
-      <c r="C37" t="s">
-        <v>15</v>
-      </c>
-      <c r="D37" t="s">
-        <v>16</v>
-      </c>
       <c r="E37">
         <v>1</v>
       </c>
       <c r="F37" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="B38" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C38" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D38" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E38">
         <v>1</v>
@@ -1424,32 +1443,32 @@
         <v>31</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="B39" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C39" t="s">
         <v>7</v>
       </c>
       <c r="D39" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E39">
         <v>1</v>
       </c>
       <c r="F39" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="B40" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C40" t="s">
         <v>7</v>
@@ -1458,38 +1477,38 @@
         <v>16</v>
       </c>
       <c r="E40">
+        <v>1</v>
+      </c>
+      <c r="F40" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>78</v>
+      </c>
+      <c r="B41" t="s">
+        <v>18</v>
+      </c>
+      <c r="C41" t="s">
+        <v>7</v>
+      </c>
+      <c r="D41" t="s">
+        <v>14</v>
+      </c>
+      <c r="E41">
         <v>2</v>
       </c>
-      <c r="F40" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
-        <v>70</v>
-      </c>
-      <c r="B41" t="s">
-        <v>24</v>
-      </c>
-      <c r="C41" t="s">
-        <v>7</v>
-      </c>
-      <c r="D41" t="s">
-        <v>8</v>
-      </c>
-      <c r="E41">
-        <v>1</v>
-      </c>
       <c r="F41" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="B42" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C42" t="s">
         <v>7</v>
@@ -1501,15 +1520,15 @@
         <v>1</v>
       </c>
       <c r="F42" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="B43" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C43" t="s">
         <v>7</v>
@@ -1521,15 +1540,15 @@
         <v>1</v>
       </c>
       <c r="F43" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="B44" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C44" t="s">
         <v>7</v>
@@ -1541,61 +1560,61 @@
         <v>1</v>
       </c>
       <c r="F44" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="B45" t="s">
         <v>6</v>
       </c>
       <c r="C45" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="D45" t="s">
-        <v>53</v>
+        <v>8</v>
       </c>
       <c r="E45">
         <v>1</v>
       </c>
       <c r="F45" t="s">
-        <v>74</v>
-      </c>
-      <c r="G45" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>77</v>
+        <v>38</v>
       </c>
       <c r="B46" t="s">
         <v>6</v>
       </c>
       <c r="C46" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D46" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="E46">
         <v>1</v>
       </c>
       <c r="F46" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+        <v>37</v>
+      </c>
+      <c r="G46" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>78</v>
+        <v>39</v>
       </c>
       <c r="B47" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="C47" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D47" t="s">
         <v>16</v>
@@ -1604,27 +1623,50 @@
         <v>1</v>
       </c>
       <c r="F47" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+        <v>37</v>
+      </c>
+      <c r="H47" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>79</v>
+        <v>40</v>
       </c>
       <c r="B48" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C48" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D48" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E48">
         <v>1</v>
       </c>
       <c r="F48" t="s">
-        <v>74</v>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>41</v>
+      </c>
+      <c r="B49" t="s">
+        <v>18</v>
+      </c>
+      <c r="C49" t="s">
+        <v>13</v>
+      </c>
+      <c r="D49" t="s">
+        <v>14</v>
+      </c>
+      <c r="E49">
+        <v>1</v>
+      </c>
+      <c r="F49" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>